<commit_message>
Update to Backbone workflow.
</commit_message>
<xml_diff>
--- a/Nomenclature comparison.xlsx
+++ b/Nomenclature comparison.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23815"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7581B982-DD7D-4506-ABB7-38E8B62443F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\TradeRES\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="First_items" sheetId="1" r:id="rId1"/>
@@ -15,9 +19,10 @@
     <sheet name="unit" sheetId="6" r:id="rId5"/>
     <sheet name="commodity_price" sheetId="7" r:id="rId6"/>
     <sheet name="node__commodity" sheetId="8" r:id="rId7"/>
-    <sheet name="Contacts" sheetId="3" r:id="rId8"/>
+    <sheet name="node__unit" sheetId="9" r:id="rId8"/>
+    <sheet name="Contacts" sheetId="3" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="129">
   <si>
     <t>First items</t>
   </si>
@@ -385,9 +390,6 @@
     <t>capacity</t>
   </si>
   <si>
-    <t>efficiency</t>
-  </si>
-  <si>
     <t>gas_turbine</t>
   </si>
   <si>
@@ -419,16 +421,28 @@
   </si>
   <si>
     <t>Hugo Algarvio, Antonio Couto, Fernando Lopes</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>efficiency_full_load</t>
+  </si>
+  <si>
+    <t>efficiency_min_load</t>
+  </si>
+  <si>
+    <t>min_load</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -806,17 +820,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
@@ -831,7 +845,7 @@
     <col min="11" max="11" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -873,7 +887,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="158.25" customHeight="1">
+    <row r="2" spans="1:18" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -915,7 +929,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="60">
+    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -957,7 +971,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="60">
+    <row r="4" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -997,7 +1011,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="45">
+    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1039,7 +1053,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="120">
+    <row r="6" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1081,7 +1095,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="150">
+    <row r="7" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1121,7 +1135,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="45">
+    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1163,7 +1177,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="30">
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1205,7 +1219,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1224,7 +1238,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1243,7 +1257,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1262,7 +1276,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1281,7 +1295,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1300,7 +1314,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1319,7 +1333,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1338,7 +1352,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="2:18">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1357,7 +1371,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="2:18">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1376,7 +1390,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="2:18">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1395,7 +1409,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="2:18">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1414,7 +1428,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="2:18">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1433,7 +1447,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="2:18">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1452,7 +1466,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="2:18">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1471,7 +1485,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="2:18">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1490,7 +1504,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="2:18">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1509,7 +1523,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="2:18">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1528,7 +1542,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="2:18">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1547,7 +1561,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="2:18">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1566,7 +1580,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="2:18">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1585,7 +1599,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="2:18">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1604,7 +1618,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="2:18">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1629,19 +1643,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDBF5A2-B094-47DB-AD35-0FA6FBFB97CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
@@ -1652,7 +1666,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>88</v>
       </c>
@@ -1663,7 +1677,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1672,7 +1686,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>33</v>
@@ -1693,7 +1707,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>89</v>
       </c>
@@ -1714,7 +1728,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -1735,7 +1749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>101</v>
       </c>
@@ -1756,7 +1770,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1765,7 +1779,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1774,7 +1788,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1783,7 +1797,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1792,7 +1806,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1801,7 +1815,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1810,7 +1824,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1819,7 +1833,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1828,7 +1842,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1837,7 +1851,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1846,7 +1860,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1855,7 +1869,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1864,7 +1878,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1879,19 +1893,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A30354-E9FE-4874-BB9F-5A6CF3E468AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1902,24 +1916,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC774D8-F270-4B5C-8910-B04C60743D85}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>108</v>
       </c>
@@ -1927,7 +1941,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -1935,7 +1949,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>110</v>
       </c>
@@ -1943,7 +1957,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>111</v>
       </c>
@@ -1951,7 +1965,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>112</v>
       </c>
@@ -1965,35 +1979,43 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0876BA35-110D-4B51-B38D-1516837B22FD}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>115</v>
-      </c>
       <c r="B2">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.4</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -2002,24 +2024,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E59A64A-EF07-4B8B-AA66-BA35C87519CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>108</v>
       </c>
@@ -2027,7 +2049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -2035,7 +2057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>110</v>
       </c>
@@ -2043,7 +2065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>111</v>
       </c>
@@ -2051,7 +2073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>112</v>
       </c>
@@ -2065,29 +2087,67 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11386AC-FDD2-4BCC-801B-419D660D21BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2095,86 +2155,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54ED6D-740E-40F7-9595-F0A81135465F}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2183,6 +2243,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031045B8A90BCED4EB320A71CA93796CA" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4bcf6570a260dba89a267bc1f6b37b5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3efa965-fed5-4637-b1ab-cbba23d8bfa1" xmlns:ns3="36631e7b-b6a2-46bf-891c-ceae7201f9ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="923283c7f088239077566491c124f9cf" ns2:_="" ns3:_="">
     <xsd:import namespace="f3efa965-fed5-4637-b1ab-cbba23d8bfa1"/>
@@ -2393,29 +2462,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FA0BFF4-EDC3-45BB-85A8-0A0213E09AFB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DF3B5A5-D1DB-49DB-A3C2-8CE71E417B40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{514AFDCB-0606-4A9C-810F-3B7B2562DB7E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FA0BFF4-EDC3-45BB-85A8-0A0213E09AFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3efa965-fed5-4637-b1ab-cbba23d8bfa1"/>
+    <ds:schemaRef ds:uri="36631e7b-b6a2-46bf-891c-ceae7201f9ee"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DF3B5A5-D1DB-49DB-A3C2-8CE71E417B40}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{514AFDCB-0606-4A9C-810F-3B7B2562DB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>